<commit_message>
24/25 Apr Source Update
</commit_message>
<xml_diff>
--- a/source-xlsx/24-04-2020.xlsx
+++ b/source-xlsx/24-04-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\covid19\source-xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D269A1B2-B009-4C28-BB0F-7FCF4484B821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C2D0DC-B1CF-4BE2-A490-FD5CC261CB33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -716,7 +716,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -724,17 +724,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1019,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1050,21 +1068,23 @@
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
-        <v>64</v>
+      <c r="C2" s="4">
+        <f>1+64</f>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="4">
+        <f>294+1</f>
         <v>295</v>
       </c>
     </row>
@@ -1072,10 +1092,10 @@
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>180</v>
       </c>
     </row>
@@ -1083,10 +1103,11 @@
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="4">
+        <f>28+9</f>
         <v>37</v>
       </c>
     </row>
@@ -1094,10 +1115,10 @@
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>12</v>
       </c>
     </row>
@@ -1105,10 +1126,10 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <f>566+19</f>
         <v>585</v>
       </c>
@@ -1117,10 +1138,10 @@
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>63</v>
       </c>
     </row>
@@ -1128,10 +1149,10 @@
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <f>141+1</f>
         <v>142</v>
       </c>
@@ -1140,10 +1161,10 @@
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1151,10 +1172,10 @@
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>8</v>
       </c>
     </row>
@@ -1162,10 +1183,10 @@
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="4">
         <v>21</v>
       </c>
     </row>
@@ -1173,10 +1194,10 @@
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1184,10 +1205,10 @@
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <v>43</v>
       </c>
     </row>
@@ -1195,10 +1216,10 @@
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="4">
         <f>45+2</f>
         <v>47</v>
       </c>
@@ -1207,10 +1228,10 @@
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="4">
         <f>6+1</f>
         <v>7</v>
       </c>
@@ -1219,10 +1240,10 @@
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <f>32+1</f>
         <v>33</v>
       </c>
@@ -1231,10 +1252,10 @@
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="4">
         <v>25</v>
       </c>
     </row>
@@ -1242,10 +1263,10 @@
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="4">
         <v>27</v>
       </c>
     </row>
@@ -1253,10 +1274,10 @@
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1264,10 +1285,10 @@
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1275,10 +1296,10 @@
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1286,10 +1307,10 @@
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="4">
         <v>10</v>
       </c>
     </row>
@@ -1297,10 +1318,10 @@
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1308,10 +1329,10 @@
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="4">
         <v>13</v>
       </c>
     </row>
@@ -1319,10 +1340,10 @@
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="4">
         <v>21</v>
       </c>
     </row>
@@ -1330,10 +1351,10 @@
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="4">
         <v>11</v>
       </c>
     </row>
@@ -1341,10 +1362,10 @@
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="4">
         <v>15</v>
       </c>
     </row>
@@ -1352,10 +1373,10 @@
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="4">
         <f>14+4</f>
         <v>18</v>
       </c>
@@ -1364,10 +1385,10 @@
       <c r="A30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="4">
         <v>10</v>
       </c>
     </row>
@@ -1375,10 +1396,10 @@
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="4">
         <v>2</v>
       </c>
     </row>
@@ -1386,10 +1407,10 @@
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="4">
         <v>5</v>
       </c>
     </row>
@@ -1397,10 +1418,10 @@
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="4">
         <v>13</v>
       </c>
     </row>
@@ -1408,10 +1429,10 @@
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1419,10 +1440,10 @@
       <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="4">
         <v>8</v>
       </c>
     </row>
@@ -1430,10 +1451,10 @@
       <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="4">
         <v>7</v>
       </c>
     </row>
@@ -1441,10 +1462,10 @@
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="4">
         <v>7</v>
       </c>
     </row>
@@ -1452,10 +1473,10 @@
       <c r="A38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1463,10 +1484,10 @@
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="4">
         <v>7</v>
       </c>
     </row>
@@ -1474,10 +1495,10 @@
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="4">
         <v>2</v>
       </c>
     </row>
@@ -1485,10 +1506,10 @@
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="4">
         <v>2</v>
       </c>
     </row>
@@ -1496,10 +1517,10 @@
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1507,10 +1528,10 @@
       <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="4">
         <f>8+1</f>
         <v>9</v>
       </c>
@@ -1519,10 +1540,10 @@
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="4">
         <v>68</v>
       </c>
     </row>
@@ -1530,10 +1551,10 @@
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="4">
         <v>30</v>
       </c>
     </row>
@@ -1541,10 +1562,10 @@
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="4">
         <v>22</v>
       </c>
     </row>
@@ -1552,10 +1573,10 @@
       <c r="A47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="4">
         <v>19</v>
       </c>
     </row>
@@ -1563,10 +1584,10 @@
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="4">
         <v>23</v>
       </c>
     </row>
@@ -1574,10 +1595,10 @@
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="4">
         <v>2</v>
       </c>
       <c r="D49" s="2"/>
@@ -1586,10 +1607,10 @@
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="4">
         <v>35</v>
       </c>
       <c r="D50" s="2"/>
@@ -1598,10 +1619,10 @@
       <c r="A51" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="4">
         <v>16</v>
       </c>
       <c r="D51" s="2"/>
@@ -1610,10 +1631,10 @@
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="4">
         <v>5</v>
       </c>
       <c r="D52" s="2"/>
@@ -1622,10 +1643,10 @@
       <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="4">
         <v>5</v>
       </c>
       <c r="D53" s="2"/>
@@ -1634,10 +1655,10 @@
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="4">
         <v>4</v>
       </c>
       <c r="D54" s="2"/>
@@ -1646,10 +1667,10 @@
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="4">
         <v>3</v>
       </c>
       <c r="D55" s="2"/>
@@ -1658,10 +1679,10 @@
       <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="4">
         <v>1</v>
       </c>
       <c r="D56" s="2"/>
@@ -1670,10 +1691,10 @@
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="4">
         <v>10</v>
       </c>
       <c r="D57" s="2"/>
@@ -1682,10 +1703,10 @@
       <c r="A58" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="4">
         <v>2</v>
       </c>
       <c r="D58" s="2"/>
@@ -1694,10 +1715,10 @@
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="4">
         <v>2</v>
       </c>
       <c r="D59" s="2"/>
@@ -1706,10 +1727,10 @@
       <c r="A60" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="4">
         <v>9</v>
       </c>
       <c r="D60" s="2"/>

</xml_diff>